<commit_message>
Worked on cohort creation script
</commit_message>
<xml_diff>
--- a/kite_codelist.xlsx
+++ b/kite_codelist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://corronallc-my.sharepoint.com/personal/ang_corevitas_com/Documents/Documents/GitHub/kite-ipet-dlbcl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{44888B14-55E4-4853-BC67-38F3B3DD8CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBA4C3AA-7536-4454-B5BD-2F6F506466D3}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{44888B14-55E4-4853-BC67-38F3B3DD8CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{419B579B-BF39-4F2C-8D44-CE295F0E4008}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="4200" windowWidth="28800" windowHeight="15225" xr2:uid="{ECF0E048-0D09-44A3-A3BB-26BE9EC47663}"/>
   </bookViews>
@@ -38,18 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="104">
   <si>
-    <t>Code type</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Variable</t>
-  </si>
-  <si>
     <t>C833</t>
   </si>
   <si>
@@ -348,6 +336,18 @@
   </si>
   <si>
     <t>opcs4</t>
+  </si>
+  <si>
+    <t>code_type</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>category</t>
   </si>
 </sst>
 </file>
@@ -406,6 +406,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -708,7 +712,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,674 +725,674 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D31" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D35" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D36" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D38" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D39" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D40" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D41" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D42" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D44" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C45" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C47" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D47" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D48" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>